<commit_message>
analysis of hospitals in Euskadi
</commit_message>
<xml_diff>
--- a/data/original/spain/euskadi/situacion-epidemiologica.xlsx
+++ b/data/original/spain/euskadi/situacion-epidemiologica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iargueso\Desktop\covid19\BERRIA\23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iargueso\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,18 +14,17 @@
   <sheets>
     <sheet name="01" sheetId="17" r:id="rId1"/>
     <sheet name="02" sheetId="14" r:id="rId2"/>
-    <sheet name="03" sheetId="15" r:id="rId3"/>
-    <sheet name="04" sheetId="16" r:id="rId4"/>
-    <sheet name="05" sheetId="13" r:id="rId5"/>
-    <sheet name="06" sheetId="11" r:id="rId6"/>
-    <sheet name="07" sheetId="12" r:id="rId7"/>
+    <sheet name="03" sheetId="16" r:id="rId3"/>
+    <sheet name="04" sheetId="13" r:id="rId4"/>
+    <sheet name="05" sheetId="11" r:id="rId5"/>
+    <sheet name="06" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="430">
   <si>
     <t>UDALERRIA / MUNICIPIO</t>
   </si>
@@ -534,9 +533,6 @@
     <t>Kasu positibo berriak Euskadin (PCR testak) / Casos positivos nuevos en Euskadi (test PCRs)</t>
   </si>
   <si>
-    <t>Intzizentzia met./ Incidencia acum.</t>
-  </si>
-  <si>
     <t xml:space="preserve">14 eguneko 100.000 biztanleko intzidentzia metatua Euskadin (PCR testak) / Incidencia acumulada 14 días en Euskadi x 100.000 habitantes (test PCRs) </t>
   </si>
   <si>
@@ -780,9 +776,6 @@
     <t>0,75</t>
   </si>
   <si>
-    <t>ZIUn ospitaleratuak / Hospitalizados en CI</t>
-  </si>
-  <si>
     <t>R0 Euskadin / R0 en Euskadi</t>
   </si>
   <si>
@@ -1246,6 +1239,81 @@
   </si>
   <si>
     <t>Desierto</t>
+  </si>
+  <si>
+    <t>2020/5/15</t>
+  </si>
+  <si>
+    <t>2020/5/16</t>
+  </si>
+  <si>
+    <t>2020/5/17</t>
+  </si>
+  <si>
+    <t>2020/5/18</t>
+  </si>
+  <si>
+    <t>2020/5/19</t>
+  </si>
+  <si>
+    <t>2020/5/20</t>
+  </si>
+  <si>
+    <t>2020/5/21</t>
+  </si>
+  <si>
+    <t>2020/5/22</t>
+  </si>
+  <si>
+    <t>2020/5/23</t>
+  </si>
+  <si>
+    <t>ZIUn ospitaleratuak / Hospitalizados en UCI</t>
+  </si>
+  <si>
+    <t>185119</t>
+  </si>
+  <si>
+    <t>106400</t>
+  </si>
+  <si>
+    <t>161700</t>
+  </si>
+  <si>
+    <t>138253</t>
+  </si>
+  <si>
+    <t>63186</t>
+  </si>
+  <si>
+    <t>13478</t>
+  </si>
+  <si>
+    <t>5914</t>
+  </si>
+  <si>
+    <t>19392</t>
+  </si>
+  <si>
+    <t>7576</t>
+  </si>
+  <si>
+    <t>17417</t>
+  </si>
+  <si>
+    <t>475</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2020/5/24</t>
+  </si>
+  <si>
+    <t>24-may.</t>
   </si>
 </sst>
 </file>
@@ -1300,14 +1368,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1"/>
@@ -1589,602 +1657,670 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" customWidth="1"/>
-    <col min="5" max="18" width="9.140625" style="4"/>
-    <col min="19" max="19" width="11.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="6"/>
+    <col min="9" max="9" width="7.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12" style="6" customWidth="1"/>
+    <col min="13" max="13" width="9" style="6" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="10" style="6" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="6" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>43966</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="P3" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>43967</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="O4" s="6" t="s">
+      <c r="S4" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="Q4" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>43968</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="L5" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="Q5" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>325</v>
-      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>43969</v>
+      <c r="A6" s="6" t="s">
+        <v>408</v>
       </c>
       <c r="B6" s="6">
         <v>166314</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>231</v>
-      </c>
       <c r="J6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>240</v>
-      </c>
       <c r="N6" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="O6" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="Q6" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="R6" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="S6" s="6" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>43970</v>
+      <c r="A7" s="6" t="s">
+        <v>409</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="M7" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="N7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>43971</v>
+      <c r="A8" s="6" t="s">
+        <v>410</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="L8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="N8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="Q8" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="R8" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>341</v>
-      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>43972</v>
+      <c r="A9" s="6" t="s">
+        <v>411</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="L9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="P9" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="Q9" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="R9" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="Q9" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>362</v>
-      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>43973</v>
+      <c r="A10" s="6" t="s">
+        <v>412</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="L10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="O10" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="N10" s="6" t="s">
+      <c r="P10" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="Q10" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="Q10" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>382</v>
-      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>43974</v>
+      <c r="A11" s="6" t="s">
+        <v>413</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="L11" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="N11" s="6" t="s">
+      <c r="P11" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="S11" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="O11" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>400</v>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2195,700 +2331,965 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B86" sqref="B3:B86"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="10">
+        <v>4.5703484022290505E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="10">
+        <v>0.18281393608916202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>96</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="10">
+        <v>0.36562787217832404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="10">
+        <v>0.54844180826748601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>102</v>
       </c>
       <c r="B7">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="10">
+        <v>1.4168080046910057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>105</v>
       </c>
       <c r="B8">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="10">
+        <v>2.6050985892705585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
       <c r="B9">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="10">
+        <v>4.1590170460284357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
       <c r="B10">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="10">
+        <v>6.3070807950760894</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
       <c r="B11">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="10">
+        <v>8.4551445441237423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>117</v>
       </c>
       <c r="B12">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="10">
+        <v>11.83720236177324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
       <c r="B13">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="10">
+        <v>15.173556695400448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
       </c>
       <c r="B14">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="10">
+        <v>19.012649353272849</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>126</v>
       </c>
       <c r="B15">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="10">
+        <v>23.720108207568771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>129</v>
       </c>
       <c r="B16">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="10">
+        <v>28.381863577842402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>132</v>
       </c>
       <c r="B17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="10">
+        <v>32.906508496049163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>135</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="10">
+        <v>37.522560382300505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
       <c r="B19">
         <v>198</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="10">
+        <v>46.389036282624858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>139</v>
       </c>
       <c r="B20">
         <v>231</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="10">
+        <v>56.763727155684805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
       <c r="B21">
         <v>269</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="10">
+        <v>68.189598161257436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>143</v>
       </c>
       <c r="B22">
         <v>335</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="10">
+        <v>82.311974724145202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>145</v>
       </c>
       <c r="B23">
         <v>320</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="10">
+        <v>95.383171154520284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>147</v>
       </c>
       <c r="B24">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="10">
+        <v>107.44889093640498</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>149</v>
       </c>
       <c r="B25">
         <v>362</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="10">
+        <v>121.84548840342649</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>151</v>
       </c>
       <c r="B26">
         <v>579</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="10">
+        <v>144.92574783468319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>153</v>
       </c>
       <c r="B27">
         <v>723</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="10">
+        <v>174.63301244917201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>155</v>
       </c>
       <c r="B28">
         <v>632</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="10">
+        <v>199.67852169338721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
       <c r="B29">
         <v>501</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="10">
+        <v>217.86850833425882</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>159</v>
       </c>
       <c r="B30">
         <v>576</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="10">
+        <v>239.53195976082452</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>161</v>
       </c>
       <c r="B31">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="10">
+        <v>246.20466842807895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>163</v>
       </c>
       <c r="B32">
         <v>327</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="10">
+        <v>256.39654536504975</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
       <c r="B33">
         <v>581</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="10">
+        <v>273.90097974558699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>91</v>
       </c>
       <c r="B34">
         <v>481</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="10">
+        <v>285.32685075115961</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
       <c r="B35">
         <v>491</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="10">
+        <v>295.47302420410813</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
       <c r="B36">
         <v>419</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="10">
+        <v>299.31211686198048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>100</v>
       </c>
       <c r="B37">
         <v>296</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="10">
+        <v>298.21523324544552</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>103</v>
       </c>
       <c r="B38">
         <v>196</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="10">
+        <v>292.9593325828821</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>106</v>
       </c>
       <c r="B39">
         <v>240</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="10">
+        <v>287.3835075321627</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>109</v>
       </c>
       <c r="B40">
         <v>416</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="10">
+        <v>279.93383963652934</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
       <c r="B41">
         <v>312</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="10">
+        <v>261.14970770336794</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>115</v>
       </c>
       <c r="B42">
         <v>279</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="10">
+        <v>245.01637784349938</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>118</v>
       </c>
       <c r="B43">
         <v>284</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="10">
+        <v>235.09872181066234</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>121</v>
       </c>
       <c r="B44">
         <v>151</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="10">
+        <v>215.67474110118889</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>124</v>
       </c>
       <c r="B45">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="10">
+        <v>211.65283450722731</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>127</v>
       </c>
       <c r="B46">
         <v>175</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="10">
+        <v>204.70590493583916</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>130</v>
       </c>
       <c r="B47">
         <v>194</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="10">
+        <v>187.01865661921275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>133</v>
       </c>
       <c r="B48">
         <v>194</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="10">
+        <v>173.90175670481537</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>136</v>
       </c>
       <c r="B49">
         <v>209</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="10">
+        <v>161.01337421052943</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>138</v>
       </c>
       <c r="B50">
         <v>125</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="10">
+        <v>147.57654990797604</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>140</v>
       </c>
       <c r="B51">
         <v>147</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="10">
+        <v>140.76673078865474</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>142</v>
       </c>
       <c r="B52">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="10">
+        <v>134.41394650955638</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>144</v>
       </c>
       <c r="B53">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="10">
+        <v>126.41583680565553</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>146</v>
       </c>
       <c r="B54">
         <v>129</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="10">
+        <v>113.29893689125815</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>148</v>
       </c>
       <c r="B55">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="10">
+        <v>104.02112963473319</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>150</v>
       </c>
       <c r="B56">
         <v>149</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="10">
+        <v>98.079676711835418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>152</v>
       </c>
       <c r="B57">
         <v>147</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="10">
+        <v>91.818299400781626</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>154</v>
       </c>
       <c r="B58">
         <v>63</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="10">
+        <v>87.796392806820052</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>156</v>
       </c>
       <c r="B59">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="10">
+        <v>82.723306080345807</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>158</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="10">
+        <v>77.421701933760119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>160</v>
       </c>
       <c r="B61">
         <v>55</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="10">
+        <v>71.068917654661732</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>162</v>
       </c>
       <c r="B62">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="10">
+        <v>66.270051832321229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>164</v>
       </c>
       <c r="B63">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="10">
+        <v>62.47666265847112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>92</v>
       </c>
       <c r="B64">
         <v>47</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="10">
+        <v>58.911790904732456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>95</v>
       </c>
       <c r="B65">
         <v>45</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="10">
+        <v>54.250035534458824</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>98</v>
       </c>
       <c r="B66">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="10">
+        <v>52.147675269433464</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>101</v>
       </c>
       <c r="B67">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="10">
+        <v>50.593756812675586</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>104</v>
       </c>
       <c r="B68">
         <v>33</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="10">
+        <v>46.206222346535696</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>107</v>
       </c>
       <c r="B69">
         <v>32</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="10">
+        <v>42.687054076819329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>110</v>
       </c>
       <c r="B70">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="10">
+        <v>38.162409158612569</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>113</v>
       </c>
       <c r="B71">
         <v>56</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="10">
+        <v>34.003392112584137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>116</v>
       </c>
       <c r="B72">
         <v>32</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="10">
+        <v>32.586584107893131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>119</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="10">
+        <v>30.895555199068379</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>122</v>
       </c>
       <c r="B74">
         <v>27</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="10">
+        <v>29.433043710355083</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>125</v>
       </c>
       <c r="B75">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="10">
+        <v>28.244753125775532</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>128</v>
       </c>
       <c r="B76">
         <v>42</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="10">
+        <v>26.096689376727877</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>131</v>
       </c>
       <c r="B77">
         <v>29</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="10">
+        <v>21.663451426565697</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>134</v>
       </c>
       <c r="B78">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="10">
+        <v>20.246643421874694</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B79">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="10">
+        <v>18.921242385228268</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B80">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" s="10">
+        <v>18.738428449139107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B81">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" s="10">
+        <v>18.052876188804749</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B82">
         <v>25</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" s="10">
+        <v>17.687248316626423</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B83">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" s="10">
+        <v>16.636068184113743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B84">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" s="10">
+        <v>14.945039275288995</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B85">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" s="10">
+        <v>12.98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B86">
         <v>9</v>
+      </c>
+      <c r="C86" s="10">
+        <v>11.93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>429</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>11.56</v>
       </c>
     </row>
   </sheetData>
@@ -2899,702 +3300,285 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="6">
+        <v>64</v>
+      </c>
+      <c r="C2" s="6">
+        <v>195423</v>
+      </c>
+      <c r="D2" s="6">
+        <v>32.749471658914253</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.3013514907665326E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="6">
+        <v>175</v>
+      </c>
+      <c r="C3" s="6">
+        <v>206343</v>
+      </c>
+      <c r="D3" s="6">
+        <v>84.810243138851334</v>
+      </c>
+      <c r="E3" s="3">
+        <v>9.0271329825647381E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1190</v>
+      </c>
+      <c r="C4" s="6">
+        <v>194050</v>
+      </c>
+      <c r="D4" s="6">
+        <v>613.2440092759598</v>
+      </c>
+      <c r="E4" s="3">
+        <v>6.1384504281440218E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1991</v>
+      </c>
+      <c r="C5" s="6">
+        <v>266369</v>
+      </c>
+      <c r="D5" s="6">
+        <v>747.45935150111313</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1027029815330651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3125</v>
+      </c>
+      <c r="C6" s="6">
+        <v>358785</v>
+      </c>
+      <c r="D6" s="6">
+        <v>870.99516423484818</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.16119880326008459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="6">
+        <v>3874</v>
+      </c>
+      <c r="C7" s="6">
+        <v>335098</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1156.0797139941151</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.19983493242546169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="11">
-        <v>4.5703484022290505E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0.18281393608916202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="11">
-        <v>0.36562787217832404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="11">
-        <v>0.54844180826748601</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="11">
-        <v>1.4168080046910057</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="11">
-        <v>2.6050985892705585</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>2602</v>
+      </c>
+      <c r="C8" s="6">
+        <v>272250</v>
+      </c>
+      <c r="D8" s="6">
+        <v>955.73921028466486</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.13422057154647685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="11">
-        <v>4.1590170460284357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2168</v>
+      </c>
+      <c r="C9" s="6">
+        <v>202172</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1072.3542330293019</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.1118332817497163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="11">
-        <v>6.3070807950760894</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2612</v>
+      </c>
+      <c r="C10" s="6">
+        <v>127540</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2047.9849458993258</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.13473640771690912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="11">
-        <v>8.4551445441237423</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1509</v>
+      </c>
+      <c r="C11" s="6">
+        <v>29987</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5032.1806115983591</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.7839678118229644E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="11">
-        <v>11.83720236177324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="11">
-        <v>15.173556695400448</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="B12">
+        <v>76</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.9203548952852574E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="11">
-        <v>19.012649353272849</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="11">
-        <v>23.720108207568771</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="11">
-        <v>28.381863577842402</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="11">
-        <v>32.906508496049163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" s="11">
-        <v>37.522560382300505</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="11">
-        <v>46.389036282624858</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="11">
-        <v>56.763727155684805</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="11">
-        <v>68.189598161257436</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="11">
-        <v>82.311974724145202</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" s="11">
-        <v>95.383171154520284</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B24" s="11">
-        <v>107.44889093640498</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="11">
-        <v>121.84548840342649</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>151</v>
-      </c>
-      <c r="B26" s="11">
-        <v>144.92574783468319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>153</v>
-      </c>
-      <c r="B27" s="11">
-        <v>174.63301244917201</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="11">
-        <v>199.67852169338721</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="11">
-        <v>217.86850833425882</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B30" s="11">
-        <v>239.53195976082452</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>161</v>
-      </c>
-      <c r="B31" s="11">
-        <v>246.20466842807895</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B32" s="11">
-        <v>256.39654536504975</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B33" s="11">
-        <v>273.90097974558699</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="11">
-        <v>285.32685075115961</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="11">
-        <v>295.47302420410813</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="11">
-        <v>299.31211686198048</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="11">
-        <v>298.21523324544552</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="11">
-        <v>292.9593325828821</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="11">
-        <v>287.3835075321627</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="11">
-        <v>279.93383963652934</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="11">
-        <v>261.14970770336794</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="11">
-        <v>245.01637784349938</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="11">
-        <v>235.09872181066234</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="11">
-        <v>215.67474110118889</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="11">
-        <v>211.65283450722731</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="11">
-        <v>204.70590493583916</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>130</v>
-      </c>
-      <c r="B47" s="11">
-        <v>187.01865661921275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>133</v>
-      </c>
-      <c r="B48" s="11">
-        <v>173.90175670481537</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>136</v>
-      </c>
-      <c r="B49" s="11">
-        <v>161.01337421052943</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>138</v>
-      </c>
-      <c r="B50" s="11">
-        <v>147.57654990797604</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" s="11">
-        <v>140.76673078865474</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>142</v>
-      </c>
-      <c r="B52" s="11">
-        <v>134.41394650955638</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>144</v>
-      </c>
-      <c r="B53" s="11">
-        <v>126.41583680565553</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" s="11">
-        <v>113.29893689125815</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>148</v>
-      </c>
-      <c r="B55" s="11">
-        <v>104.02112963473319</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>150</v>
-      </c>
-      <c r="B56" s="11">
-        <v>98.079676711835418</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57" s="11">
-        <v>91.818299400781626</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>154</v>
-      </c>
-      <c r="B58" s="11">
-        <v>87.796392806820052</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>156</v>
-      </c>
-      <c r="B59" s="11">
-        <v>82.723306080345807</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>158</v>
-      </c>
-      <c r="B60" s="11">
-        <v>77.421701933760119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>160</v>
-      </c>
-      <c r="B61" s="11">
-        <v>71.068917654661732</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>162</v>
-      </c>
-      <c r="B62" s="11">
-        <v>66.270051832321229</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>164</v>
-      </c>
-      <c r="B63" s="11">
-        <v>62.47666265847112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="11">
-        <v>58.911790904732456</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>95</v>
-      </c>
-      <c r="B65" s="11">
-        <v>54.250035534458824</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>98</v>
-      </c>
-      <c r="B66" s="11">
-        <v>52.147675269433464</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" s="11">
-        <v>50.593756812675586</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>104</v>
-      </c>
-      <c r="B68" s="11">
-        <v>46.206222346535696</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>107</v>
-      </c>
-      <c r="B69" s="11">
-        <v>42.687054076819329</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="11">
-        <v>38.162409158612569</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>113</v>
-      </c>
-      <c r="B71" s="11">
-        <v>34.003392112584137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>116</v>
-      </c>
-      <c r="B72" s="11">
-        <v>32.586584107893131</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" s="11">
-        <v>30.895555199068379</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" s="11">
-        <v>29.433043710355083</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>125</v>
-      </c>
-      <c r="B75" s="11">
-        <v>28.244753125775532</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="11">
-        <v>26.096689376727877</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>131</v>
-      </c>
-      <c r="B77" s="11">
-        <v>21.663451426565697</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>134</v>
-      </c>
-      <c r="B78" s="11">
-        <v>20.246643421874694</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>186</v>
-      </c>
-      <c r="B79" s="11">
-        <v>18.921242385228268</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>201</v>
-      </c>
-      <c r="B80" s="11">
-        <v>18.738428449139107</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>207</v>
-      </c>
-      <c r="B81" s="11">
-        <v>18.052876188804749</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>270</v>
-      </c>
-      <c r="B82" s="11">
-        <v>17.687248316626423</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>342</v>
-      </c>
-      <c r="B83" s="11">
-        <v>16.636068184113743</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>363</v>
-      </c>
-      <c r="B84" s="11">
-        <v>14.945039275288995</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>383</v>
-      </c>
-      <c r="B85" s="11">
-        <v>12.98</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>401</v>
-      </c>
-      <c r="B86" s="11">
-        <v>11.93</v>
-      </c>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3603,298 +3587,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="6">
-        <v>64</v>
-      </c>
-      <c r="C2" s="6">
-        <v>195423</v>
-      </c>
-      <c r="D2" s="6">
-        <v>32.749471658914253</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3.3013514907665326E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="6">
-        <v>175</v>
-      </c>
-      <c r="C3" s="6">
-        <v>206343</v>
-      </c>
-      <c r="D3" s="6">
-        <v>84.810243138851334</v>
-      </c>
-      <c r="E3" s="3">
-        <v>9.0271329825647381E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1190</v>
-      </c>
-      <c r="C4" s="6">
-        <v>194050</v>
-      </c>
-      <c r="D4" s="6">
-        <v>613.2440092759598</v>
-      </c>
-      <c r="E4" s="3">
-        <v>6.1384504281440218E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1991</v>
-      </c>
-      <c r="C5" s="6">
-        <v>266369</v>
-      </c>
-      <c r="D5" s="6">
-        <v>747.45935150111313</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.1027029815330651</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="6">
-        <v>3125</v>
-      </c>
-      <c r="C6" s="6">
-        <v>358785</v>
-      </c>
-      <c r="D6" s="6">
-        <v>870.99516423484818</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.16119880326008459</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="6">
-        <v>3874</v>
-      </c>
-      <c r="C7" s="6">
-        <v>335098</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1156.0797139941151</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.19983493242546169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2602</v>
-      </c>
-      <c r="C8" s="6">
-        <v>272250</v>
-      </c>
-      <c r="D8" s="6">
-        <v>955.73921028466486</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.13422057154647685</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="6">
-        <v>2168</v>
-      </c>
-      <c r="C9" s="6">
-        <v>202172</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1072.3542330293019</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.1118332817497163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2612</v>
-      </c>
-      <c r="C10" s="6">
-        <v>127540</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2047.9849458993258</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.13473640771690912</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1509</v>
-      </c>
-      <c r="C11" s="6">
-        <v>29987</v>
-      </c>
-      <c r="D11" s="6">
-        <v>5032.1806115983591</v>
-      </c>
-      <c r="E11" s="3">
-        <v>7.7839678118229644E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B12">
-        <v>76</v>
-      </c>
-      <c r="E12" s="3">
-        <v>3.9203548952852574E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3906,16 +3601,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
         <v>174</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>176</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4098,12 +3793,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4165,13 +3860,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4189,37 +3882,37 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" t="s">
         <v>274</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" t="s">
         <v>275</v>
       </c>
-      <c r="G2" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>345</v>
+      <c r="I2" s="9" t="s">
+        <v>343</v>
       </c>
       <c r="J2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4262,7 +3955,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4300,7 +3993,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4338,7 +4031,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4490,7 +4183,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4528,7 +4221,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -4566,7 +4259,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -4639,7 +4332,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4677,7 +4370,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4905,7 +4598,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4943,7 +4636,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -5209,7 +4902,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5437,7 +5130,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5475,7 +5168,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5513,7 +5206,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5589,7 +5282,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B39">
         <v>31</v>
@@ -5665,7 +5358,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -5703,7 +5396,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -5779,7 +5472,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -5855,7 +5548,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -5893,7 +5586,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -5969,7 +5662,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -6052,12 +5745,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6070,45 +5763,45 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C2" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>345</v>
+      <c r="I2" s="8" t="s">
+        <v>343</v>
       </c>
       <c r="J2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6189,7 +5882,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6227,7 +5920,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6303,7 +5996,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6379,7 +6072,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6417,7 +6110,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6455,7 +6148,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6493,7 +6186,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6531,7 +6224,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6569,7 +6262,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -6721,7 +6414,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -6911,7 +6604,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -7025,7 +6718,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -7291,7 +6984,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -7405,7 +7098,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -7519,7 +7212,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -7709,7 +7402,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -7899,7 +7592,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -7975,7 +7668,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -8469,7 +8162,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -8545,7 +8238,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -8659,7 +8352,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -8735,7 +8428,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -8773,7 +8466,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -8811,7 +8504,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -8887,7 +8580,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -8925,7 +8618,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B77">
         <v>0</v>

</xml_diff>

<commit_message>
update Euskadi charts and data 2020.05.30. Remove mistaken chart 100% has mistaken calculation
</commit_message>
<xml_diff>
--- a/data/original/spain/euskadi/situacion-epidemiologica.xlsx
+++ b/data/original/spain/euskadi/situacion-epidemiologica.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iargueso\Desktop\covid19\BERRIA\29\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iargueso\Desktop\covid19\BERRIA\30\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="17" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="06" sheetId="18" r:id="rId6"/>
     <sheet name="07" sheetId="19" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="986">
   <si>
     <t>UDALERRIA / MUNICIPIO</t>
   </si>
@@ -2931,7 +2931,58 @@
     <t>Ermua</t>
   </si>
   <si>
+    <t>2020/5/30</t>
+  </si>
+  <si>
+    <t>201970</t>
+  </si>
+  <si>
+    <t>113650</t>
+  </si>
+  <si>
+    <t>177460</t>
+  </si>
+  <si>
+    <t>150863</t>
+  </si>
+  <si>
+    <t>68950</t>
+  </si>
+  <si>
+    <t>13518</t>
+  </si>
+  <si>
+    <t>6302</t>
+  </si>
+  <si>
+    <t>19820</t>
+  </si>
+  <si>
+    <t>3006</t>
+  </si>
+  <si>
+    <t>7610</t>
+  </si>
+  <si>
+    <t>16499</t>
+  </si>
+  <si>
+    <t>1780</t>
+  </si>
+  <si>
+    <t>1541</t>
+  </si>
+  <si>
     <t>29-may.</t>
+  </si>
+  <si>
+    <t>30-may.</t>
+  </si>
+  <si>
+    <t>30/05</t>
+  </si>
+  <si>
+    <t>Zaramaga</t>
   </si>
 </sst>
 </file>
@@ -3037,7 +3088,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office gaia">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3299,7 +3350,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:S99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6638,6 +6689,65 @@
         <v>328</v>
       </c>
     </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>968</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>969</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>970</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>973</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>974</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>975</v>
+      </c>
+      <c r="I99" s="6" t="s">
+        <v>976</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>977</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>978</v>
+      </c>
+      <c r="L99" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="M99" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="N99" s="6" t="s">
+        <v>979</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="P99" s="6" t="s">
+        <v>981</v>
+      </c>
+      <c r="Q99" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="R99" s="6" t="s">
+        <v>854</v>
+      </c>
+      <c r="S99" s="6" t="s">
+        <v>925</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6646,7 +6756,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7653,13 +7763,24 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>968</v>
+        <v>982</v>
       </c>
       <c r="B92">
         <v>7</v>
       </c>
       <c r="C92" s="10">
         <v>6.6270051832321233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>983</v>
+      </c>
+      <c r="B93">
+        <v>5</v>
+      </c>
+      <c r="C93" s="10">
+        <v>6.12</v>
       </c>
     </row>
   </sheetData>
@@ -7672,7 +7793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7681,8 +7804,8 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7717,19 +7840,19 @@
         <v>43</v>
       </c>
       <c r="B2" s="6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="6">
         <v>195423</v>
       </c>
       <c r="D2" s="6">
-        <v>35.819734626937461</v>
+        <v>36.331445121607999</v>
       </c>
       <c r="E2" s="3">
-        <v>3.5341041046094814E-3</v>
+        <v>3.5822401614530779E-3</v>
       </c>
       <c r="F2" s="6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="6">
         <v>0</v>
@@ -7752,7 +7875,7 @@
         <v>94.987472315513486</v>
       </c>
       <c r="E3" s="3">
-        <v>9.8954914929065482E-3</v>
+        <v>9.8890010090817351E-3</v>
       </c>
       <c r="F3" s="6">
         <v>196</v>
@@ -7769,25 +7892,25 @@
         <v>44</v>
       </c>
       <c r="B4" s="6">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="C4" s="6">
         <v>194050</v>
       </c>
       <c r="D4" s="6">
-        <v>628.18861118268489</v>
+        <v>628.70394228291673</v>
       </c>
       <c r="E4" s="3">
-        <v>6.15438986216994E-2</v>
+        <v>6.1553985872855703E-2</v>
       </c>
       <c r="F4" s="6">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G4" s="6">
         <v>2</v>
       </c>
       <c r="H4" s="3">
-        <v>1.6406890894175555E-3</v>
+        <v>1.639344262295082E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7804,7 +7927,7 @@
         <v>765.47946645442971</v>
       </c>
       <c r="E5" s="3">
-        <v>0.10294340384712475</v>
+        <v>0.10287588294651867</v>
       </c>
       <c r="F5" s="6">
         <v>2039</v>
@@ -7821,25 +7944,25 @@
         <v>46</v>
       </c>
       <c r="B6" s="6">
-        <v>3211</v>
+        <v>3218</v>
       </c>
       <c r="C6" s="6">
         <v>358785</v>
       </c>
       <c r="D6" s="6">
-        <v>894.96495115459118</v>
+        <v>896.91598032247725</v>
       </c>
       <c r="E6" s="3">
-        <v>0.16211440399858637</v>
+        <v>0.16236125126135217</v>
       </c>
       <c r="F6" s="6">
-        <v>3211</v>
+        <v>3218</v>
       </c>
       <c r="G6" s="6">
         <v>11</v>
       </c>
       <c r="H6" s="3">
-        <v>3.425724073497353E-3</v>
+        <v>3.4182722187694218E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -7856,7 +7979,7 @@
         <v>1190.0996126506275</v>
       </c>
       <c r="E7" s="3">
-        <v>0.20134295955975159</v>
+        <v>0.2012108980827447</v>
       </c>
       <c r="F7" s="6">
         <v>3988</v>
@@ -7873,25 +7996,25 @@
         <v>136</v>
       </c>
       <c r="B8" s="6">
-        <v>2658</v>
+        <v>2660</v>
       </c>
       <c r="C8" s="6">
         <v>272250</v>
       </c>
       <c r="D8" s="6">
-        <v>976.3085399449036</v>
+        <v>977.04315886134066</v>
       </c>
       <c r="E8" s="3">
-        <v>0.13419498157217147</v>
+        <v>0.13420787083753785</v>
       </c>
       <c r="F8" s="6">
-        <v>2658</v>
+        <v>2660</v>
       </c>
       <c r="G8" s="6">
         <v>108</v>
       </c>
       <c r="H8" s="3">
-        <v>4.0632054176072234E-2</v>
+        <v>4.06015037593985E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7908,16 +8031,16 @@
         <v>1085.2145697722731</v>
       </c>
       <c r="E9" s="3">
-        <v>0.11076892007876003</v>
+        <v>0.11069626639757821</v>
       </c>
       <c r="F9" s="6">
         <v>2194</v>
       </c>
       <c r="G9" s="6">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="H9" s="3">
-        <v>0.1349134001823154</v>
+        <v>0.13628076572470374</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7925,25 +8048,25 @@
         <v>49</v>
       </c>
       <c r="B10" s="6">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="C10" s="6">
         <v>127540</v>
       </c>
       <c r="D10" s="6">
-        <v>2069.1547749725578</v>
+        <v>2070.7229104594635</v>
       </c>
       <c r="E10" s="3">
-        <v>0.13323572474377746</v>
+        <v>0.1332492431886983</v>
       </c>
       <c r="F10" s="6">
-        <v>2639</v>
+        <v>2641</v>
       </c>
       <c r="G10" s="6">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="H10" s="3">
-        <v>0.23645320197044334</v>
+        <v>0.23703142748958728</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7960,7 +8083,7 @@
         <v>5048.854503618235</v>
       </c>
       <c r="E11" s="3">
-        <v>7.6437623062553639E-2</v>
+        <v>7.6387487386478312E-2</v>
       </c>
       <c r="F11" s="6">
         <v>1514</v>
@@ -7980,7 +8103,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="3">
-        <v>3.9884889180592719E-3</v>
+        <v>3.9858728557013116E-3</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -7989,25 +8112,25 @@
         <v>50</v>
       </c>
       <c r="B13">
-        <v>19807</v>
+        <v>19820</v>
       </c>
       <c r="C13">
         <v>2188017</v>
       </c>
       <c r="D13">
-        <v>905.24890802950802</v>
+        <v>905.84305332179781</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>19807</v>
+        <v>19820</v>
       </c>
       <c r="G13">
-        <v>1536</v>
+        <v>1541</v>
       </c>
       <c r="H13" s="3">
-        <v>7.7548341495430911E-2</v>
+        <v>7.7749747729566096E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -8101,7 +8224,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8111,12 +8234,12 @@
     <col min="2" max="8" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8171,8 +8294,11 @@
       <c r="R2" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8227,8 +8353,11 @@
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>331</v>
       </c>
@@ -8283,8 +8412,11 @@
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -8339,8 +8471,11 @@
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>313</v>
       </c>
@@ -8395,8 +8530,11 @@
       <c r="R6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -8451,8 +8589,11 @@
       <c r="R7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -8507,8 +8648,11 @@
       <c r="R8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -8563,8 +8707,11 @@
       <c r="R9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>232</v>
       </c>
@@ -8619,8 +8766,11 @@
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>293</v>
       </c>
@@ -8675,8 +8825,11 @@
       <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -8731,8 +8884,11 @@
       <c r="R12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>168</v>
       </c>
@@ -8787,8 +8943,11 @@
       <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>294</v>
       </c>
@@ -8843,8 +9002,11 @@
       <c r="R14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -8899,8 +9061,11 @@
       <c r="R15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8955,8 +9120,11 @@
       <c r="R16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -9011,8 +9179,11 @@
       <c r="R17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -9067,8 +9238,11 @@
       <c r="R18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -9123,8 +9297,11 @@
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -9179,8 +9356,11 @@
       <c r="R20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>170</v>
       </c>
@@ -9235,8 +9415,11 @@
       <c r="R21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>552</v>
       </c>
@@ -9291,8 +9474,11 @@
       <c r="R22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -9347,8 +9533,11 @@
       <c r="R23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -9403,8 +9592,11 @@
       <c r="R24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -9459,8 +9651,11 @@
       <c r="R25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -9515,8 +9710,11 @@
       <c r="R26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -9571,8 +9769,11 @@
       <c r="R27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -9627,8 +9828,11 @@
       <c r="R28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -9683,8 +9887,11 @@
       <c r="R29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -9739,8 +9946,11 @@
       <c r="R30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -9795,8 +10005,11 @@
       <c r="R31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>484</v>
       </c>
@@ -9851,8 +10064,11 @@
       <c r="R32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -9907,8 +10123,11 @@
       <c r="R33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -9963,8 +10182,11 @@
       <c r="R34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -10019,8 +10241,11 @@
       <c r="R35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -10075,8 +10300,11 @@
       <c r="R36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>233</v>
       </c>
@@ -10131,8 +10359,11 @@
       <c r="R37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -10187,8 +10418,11 @@
       <c r="R38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -10243,8 +10477,11 @@
       <c r="R39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -10299,8 +10536,11 @@
       <c r="R40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -10355,8 +10595,11 @@
       <c r="R41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -10411,8 +10654,11 @@
       <c r="R42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -10467,8 +10713,11 @@
       <c r="R43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -10523,8 +10772,11 @@
       <c r="R44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -10579,8 +10831,11 @@
       <c r="R45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>234</v>
       </c>
@@ -10635,8 +10890,11 @@
       <c r="R46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>157</v>
       </c>
@@ -10691,8 +10949,11 @@
       <c r="R47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -10747,8 +11008,11 @@
       <c r="R48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -10801,6 +11065,9 @@
         <v>0</v>
       </c>
       <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
         <v>0</v>
       </c>
     </row>
@@ -10815,7 +11082,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10827,12 +11094,12 @@
     <col min="7" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>858</v>
       </c>
@@ -10887,8 +11154,11 @@
       <c r="R2" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>860</v>
       </c>
@@ -10943,8 +11213,11 @@
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>861</v>
       </c>
@@ -10999,8 +11272,11 @@
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>862</v>
       </c>
@@ -11055,8 +11331,11 @@
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>863</v>
       </c>
@@ -11111,8 +11390,11 @@
       <c r="R6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>864</v>
       </c>
@@ -11167,8 +11449,11 @@
       <c r="R7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>865</v>
       </c>
@@ -11223,8 +11508,11 @@
       <c r="R8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>866</v>
       </c>
@@ -11279,8 +11567,11 @@
       <c r="R9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>867</v>
       </c>
@@ -11335,8 +11626,11 @@
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>868</v>
       </c>
@@ -11391,8 +11685,11 @@
       <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>869</v>
       </c>
@@ -11447,8 +11744,11 @@
       <c r="R12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>870</v>
       </c>
@@ -11503,8 +11803,11 @@
       <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>871</v>
       </c>
@@ -11559,8 +11862,11 @@
       <c r="R14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>872</v>
       </c>
@@ -11615,8 +11921,11 @@
       <c r="R15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>873</v>
       </c>
@@ -11671,8 +11980,11 @@
       <c r="R16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>874</v>
       </c>
@@ -11727,8 +12039,11 @@
       <c r="R17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>875</v>
       </c>
@@ -11783,8 +12098,11 @@
       <c r="R18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>876</v>
       </c>
@@ -11839,8 +12157,11 @@
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>877</v>
       </c>
@@ -11895,8 +12216,11 @@
       <c r="R20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>878</v>
       </c>
@@ -11951,8 +12275,11 @@
       <c r="R21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>879</v>
       </c>
@@ -12007,8 +12334,11 @@
       <c r="R22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>880</v>
       </c>
@@ -12063,8 +12393,11 @@
       <c r="R23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>881</v>
       </c>
@@ -12119,8 +12452,11 @@
       <c r="R24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>882</v>
       </c>
@@ -12175,8 +12511,11 @@
       <c r="R25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>883</v>
       </c>
@@ -12231,8 +12570,11 @@
       <c r="R26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>884</v>
       </c>
@@ -12287,8 +12629,11 @@
       <c r="R27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>967</v>
       </c>
@@ -12343,8 +12688,11 @@
       <c r="R28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>885</v>
       </c>
@@ -12399,8 +12747,11 @@
       <c r="R29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>886</v>
       </c>
@@ -12455,8 +12806,11 @@
       <c r="R30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>887</v>
       </c>
@@ -12511,8 +12865,11 @@
       <c r="R31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>888</v>
       </c>
@@ -12567,8 +12924,11 @@
       <c r="R32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>928</v>
       </c>
@@ -12623,8 +12983,11 @@
       <c r="R33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>889</v>
       </c>
@@ -12679,8 +13042,11 @@
       <c r="R34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>890</v>
       </c>
@@ -12735,8 +13101,11 @@
       <c r="R35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>891</v>
       </c>
@@ -12791,8 +13160,11 @@
       <c r="R36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>892</v>
       </c>
@@ -12847,8 +13219,11 @@
       <c r="R37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>893</v>
       </c>
@@ -12903,8 +13278,11 @@
       <c r="R38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>894</v>
       </c>
@@ -12959,8 +13337,11 @@
       <c r="R39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>895</v>
       </c>
@@ -13015,8 +13396,11 @@
       <c r="R40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>896</v>
       </c>
@@ -13071,8 +13455,11 @@
       <c r="R41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>897</v>
       </c>
@@ -13127,8 +13514,11 @@
       <c r="R42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>898</v>
       </c>
@@ -13183,8 +13573,11 @@
       <c r="R43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>899</v>
       </c>
@@ -13239,8 +13632,11 @@
       <c r="R44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>900</v>
       </c>
@@ -13295,8 +13691,11 @@
       <c r="R45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>901</v>
       </c>
@@ -13351,8 +13750,11 @@
       <c r="R46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>902</v>
       </c>
@@ -13407,8 +13809,11 @@
       <c r="R47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>903</v>
       </c>
@@ -13463,8 +13868,11 @@
       <c r="R48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>904</v>
       </c>
@@ -13519,8 +13927,11 @@
       <c r="R49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>905</v>
       </c>
@@ -13575,8 +13986,11 @@
       <c r="R50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>906</v>
       </c>
@@ -13631,8 +14045,11 @@
       <c r="R51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>907</v>
       </c>
@@ -13687,8 +14104,11 @@
       <c r="R52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>908</v>
       </c>
@@ -13743,8 +14163,11 @@
       <c r="R53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -13799,8 +14222,11 @@
       <c r="R54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>909</v>
       </c>
@@ -13855,8 +14281,11 @@
       <c r="R55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>
@@ -13911,8 +14340,11 @@
       <c r="R56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>28</v>
       </c>
@@ -13967,8 +14399,11 @@
       <c r="R57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -14023,8 +14458,11 @@
       <c r="R58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -14079,8 +14517,11 @@
       <c r="R59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -14135,8 +14576,11 @@
       <c r="R60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>52</v>
       </c>
@@ -14191,8 +14635,11 @@
       <c r="R61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -14247,8 +14694,11 @@
       <c r="R62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -14303,8 +14753,11 @@
       <c r="R63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -14359,8 +14812,11 @@
       <c r="R64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -14415,8 +14871,11 @@
       <c r="R65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -14471,8 +14930,11 @@
       <c r="R66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>37</v>
       </c>
@@ -14527,8 +14989,11 @@
       <c r="R67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>332</v>
       </c>
@@ -14583,8 +15048,11 @@
       <c r="R68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>53</v>
       </c>
@@ -14639,8 +15107,11 @@
       <c r="R69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -14695,8 +15166,11 @@
       <c r="R70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -14751,8 +15225,11 @@
       <c r="R71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -14807,8 +15284,11 @@
       <c r="R72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -14863,8 +15343,11 @@
       <c r="R73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -14919,8 +15402,11 @@
       <c r="R74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>333</v>
       </c>
@@ -14975,8 +15461,11 @@
       <c r="R75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>160</v>
       </c>
@@ -15031,284 +15520,331 @@
       <c r="R76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>985</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>171</v>
       </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-      <c r="M77">
-        <v>0</v>
-      </c>
-      <c r="N77">
-        <v>0</v>
-      </c>
-      <c r="O77">
-        <v>0</v>
-      </c>
-      <c r="P77">
-        <v>0</v>
-      </c>
-      <c r="Q77">
-        <v>0</v>
-      </c>
-      <c r="R77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>41</v>
       </c>
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-      <c r="N78">
-        <v>0</v>
-      </c>
-      <c r="O78">
-        <v>1</v>
-      </c>
-      <c r="P78">
-        <v>0</v>
-      </c>
-      <c r="Q78">
-        <v>0</v>
-      </c>
-      <c r="R78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>161</v>
       </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-      <c r="M79">
-        <v>0</v>
-      </c>
-      <c r="N79">
-        <v>0</v>
-      </c>
-      <c r="O79">
-        <v>0</v>
-      </c>
-      <c r="P79">
-        <v>0</v>
-      </c>
-      <c r="Q79">
-        <v>0</v>
-      </c>
-      <c r="R79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>235</v>
       </c>
-      <c r="B80">
-        <v>0</v>
-      </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
-      <c r="M80">
-        <v>0</v>
-      </c>
-      <c r="N80">
-        <v>0</v>
-      </c>
-      <c r="O80">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
         <v>2</v>
       </c>
-      <c r="P80">
-        <v>0</v>
-      </c>
-      <c r="Q80">
-        <v>0</v>
-      </c>
-      <c r="R80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>42</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>4</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>2</v>
       </c>
-      <c r="D81">
+      <c r="D82">
         <v>3</v>
       </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81">
-        <v>1</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81">
-        <v>0</v>
-      </c>
-      <c r="J81">
-        <v>1</v>
-      </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
-      <c r="M81">
-        <v>0</v>
-      </c>
-      <c r="N81">
-        <v>0</v>
-      </c>
-      <c r="O81">
-        <v>0</v>
-      </c>
-      <c r="P81">
-        <v>0</v>
-      </c>
-      <c r="Q81">
-        <v>0</v>
-      </c>
-      <c r="R81">
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82">
         <v>0</v>
       </c>
     </row>
@@ -15321,15 +15857,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="14" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="15" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="14"/>
   </cols>
@@ -18457,9 +18991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>